<commit_message>
Fix for case sensitivity
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/dup_col_names.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/dup_col_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgivre/github/drill-dev/drill/contrib/format-excel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73F2A197-27EA-E846-9E77-FEB508A4A58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40D6721-C735-5E4E-9EA2-AB13C0A0B0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{2848CA15-442F-7644-A64A-5A9923F23510}"/>
   </bookViews>
@@ -34,12 +34,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Col1</t>
   </si>
   <si>
     <t>Col1_1</t>
+  </si>
+  <si>
+    <t>column1</t>
+  </si>
+  <si>
+    <t>COLUMN1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -391,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14161214-827D-2545-82A9-387DE3E26BAB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +442,14 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -426,8 +462,14 @@
       <c r="D2">
         <v>13</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -440,8 +482,14 @@
       <c r="D3">
         <v>14</v>
       </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -454,8 +502,14 @@
       <c r="D4">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -467,6 +521,12 @@
       </c>
       <c r="D5">
         <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>